<commit_message>
remove same loops from main file to log_f
</commit_message>
<xml_diff>
--- a/eq_log/80001110.xlsx
+++ b/eq_log/80001110.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>інше</t>
+  </si>
+  <si>
+    <t>31/01/2018</t>
+  </si>
+  <si>
+    <t>Зазубрини в місті відрізу контакту</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>**</t>
@@ -627,27 +636,21 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8"/>
-    <row r="9" spans="1:8"/>
-    <row r="10" spans="1:8"/>
-    <row r="11" spans="1:8"/>
-    <row r="12" spans="1:8"/>
-    <row r="13" spans="1:8"/>
-    <row r="14" spans="1:8"/>
-    <row r="15" spans="1:8"/>
-    <row r="16" spans="1:8"/>
-    <row r="17" spans="1:8"/>
-    <row r="18" spans="1:8"/>
-    <row r="19" spans="1:8"/>
-    <row r="20" spans="1:8"/>
-    <row r="21" spans="1:8"/>
-    <row r="22" spans="1:8"/>
-    <row r="23" spans="1:8"/>
-    <row r="24" spans="1:8"/>
-    <row r="25" spans="1:8"/>
-    <row r="26" spans="1:8"/>
-    <row r="27" spans="1:8"/>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="28" spans="1:8">
       <c r="H28" s="1" t="n"/>
     </row>

</xml_diff>

<commit_message>
refactoring of code and uncomment of spare parts windows
</commit_message>
<xml_diff>
--- a/eq_log/80001110.xlsx
+++ b/eq_log/80001110.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="555" windowWidth="15975" windowHeight="9915"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Не відповідне термоусадження</t>
   </si>
   <si>
-    <t>896325741</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>інше</t>
   </si>
   <si>
@@ -61,7 +55,10 @@
     <t>Зазубрини в місті відрізу контакту</t>
   </si>
   <si>
-    <t>6</t>
+    <t>07/02/2018</t>
+  </si>
+  <si>
+    <t>Пошкодження поверхні контакту</t>
   </si>
   <si>
     <t>**</t>
@@ -71,50 +68,49 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="20"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -127,13 +123,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,55 +191,56 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
-    <cellStyle builtinId="8" name="Гиперссылка" xfId="1"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -531,36 +528,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="15" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="15" width="21"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="15" width="34.85546875"/>
-    <col customWidth="1" max="5" min="4" style="15" width="23.7109375"/>
-    <col customWidth="1" max="6" min="6" style="16" width="23.7109375"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="16" width="11.28515625"/>
+    <col min="1" max="1" width="10.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26.25" r="1" s="16" spans="1:8">
-      <c r="A1" s="14" t="n">
+    <row r="1" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A1" s="14">
         <v>80001110</v>
       </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="29.45" r="2" s="16" spans="1:8">
+    <row r="2" spans="1:7" ht="29.45" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -576,22 +574,22 @@
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="n"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="9" t="n"/>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="15" t="n"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="15" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="3"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -600,11 +598,11 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -614,11 +612,11 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -626,39 +624,53 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="H28" s="1" t="n"/>
+    <row r="28" spans="8:8">
+      <c r="H28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add write data togeneral log file
</commit_message>
<xml_diff>
--- a/eq_log/80001110.xlsx
+++ b/eq_log/80001110.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>середне значення циклів між замінами</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -234,6 +237,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -532,7 +538,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -543,9 +549,10 @@
     <col min="4" max="5" width="23.7109375" style="12" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" style="13" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" customHeight="1">
+    <row r="1" spans="1:8" ht="26.25" customHeight="1">
       <c r="A1" s="14">
         <v>80001110</v>
       </c>
@@ -557,8 +564,11 @@
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="29.45" customHeight="1">
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.45" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -578,8 +588,11 @@
       <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="17">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="9"/>
       <c r="C3" s="2"/>
@@ -588,7 +601,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -602,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -616,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -630,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -644,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -658,7 +671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>

</xml_diff>